<commit_message>
[update] adicionales eae y aod filter
</commit_message>
<xml_diff>
--- a/alta_floresta_daily.xlsx
+++ b/alta_floresta_daily.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\algoritmo clasificación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\algoritmo clasificación\AERCLASS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,9 +33,6 @@
     <t>aod440</t>
   </si>
   <si>
-    <t>eae440_870</t>
-  </si>
-  <si>
     <t>fmf500</t>
   </si>
   <si>
@@ -52,6 +49,9 @@
   </si>
   <si>
     <t>rri440</t>
+  </si>
+  <si>
+    <t>eae</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
   <dimension ref="A1:K1559"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,7 +442,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -454,22 +454,22 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>